<commit_message>
commit de fin de journée
Ajout de l'analyse fonctionnelle dans la documentation

Création des maquettes

Mise à jour du planning effectif
</commit_message>
<xml_diff>
--- a/doc/Planning.xlsx
+++ b/doc/Planning.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Ecole\CFC\TPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SAUSERR_INFO\Documents\GitHub\SimpleTab\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>Analyse</t>
   </si>
@@ -43,11 +43,14 @@
   <si>
     <t>Implémentation Code</t>
   </si>
+  <si>
+    <t>Planning effectif</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,7 +81,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -223,11 +226,127 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -242,20 +361,28 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,63 +677,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="15"/>
+      <c r="A1" s="13"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
@@ -699,10 +826,10 @@
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="7"/>
-      <c r="K10" s="13"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="8"/>
@@ -713,27 +840,169 @@
       <c r="G11" s="9"/>
       <c r="H11" s="8"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="12"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
+      <c r="A12" s="14"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="15"/>
+      <c r="A13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="15"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A14" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+    </row>
+    <row r="17" spans="1:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="4">
+        <v>1</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3</v>
+      </c>
+      <c r="E17" s="5">
+        <v>4</v>
+      </c>
+      <c r="F17" s="4">
+        <v>5</v>
+      </c>
+      <c r="G17" s="5">
+        <v>6</v>
+      </c>
+      <c r="H17" s="4">
+        <v>7</v>
+      </c>
+      <c r="I17" s="5">
+        <v>8</v>
+      </c>
+      <c r="J17" s="4">
+        <v>9</v>
+      </c>
+      <c r="K17" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="23"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="23"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="23"/>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="25"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:K5"/>
     <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A14:K16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>